<commit_message>
Added appendix D, general edditing
</commit_message>
<xml_diff>
--- a/Written Report/Part List.xlsx
+++ b/Written Report/Part List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Purchased Parts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
   <si>
     <t>Part Number</t>
   </si>
@@ -198,7 +198,82 @@
     <t>scrap</t>
   </si>
   <si>
-    <t>X</t>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>Material Number</t>
+  </si>
+  <si>
+    <t>PLA Fillament</t>
+  </si>
+  <si>
+    <t>MSU Makerspace</t>
+  </si>
+  <si>
+    <t>4 parts</t>
+  </si>
+  <si>
+    <t>10 ft 1"x2"x1/8" 6063-T52 Aluminum Rectangular Tube</t>
+  </si>
+  <si>
+    <t>Midwest Steel and Aluminum</t>
+  </si>
+  <si>
+    <t>3/16" 6061 Aluminum Plate 2'x3'</t>
+  </si>
+  <si>
+    <t>The Metal Store</t>
+  </si>
+  <si>
+    <t>2"x2"x1' 6061 Aluminum Square Bar</t>
+  </si>
+  <si>
+    <t>Metals Depot</t>
+  </si>
+  <si>
+    <t>1/2" 1018 Cold Finish Steel Round 4ft length</t>
+  </si>
+  <si>
+    <t>5/8" 1018 Cold Finish Steel Round 2ft length</t>
+  </si>
+  <si>
+    <t>3/8"x4"x2' A-36 Steel Flat</t>
   </si>
 </sst>
 </file>
@@ -230,7 +305,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -238,32 +313,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,405 +695,424 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="12">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="14">
         <v>11600</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="11">
         <v>3400</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="12">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -988,12 +1121,257 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>